<commit_message>
updtaed awardees wireframe pdf
</commit_message>
<xml_diff>
--- a/design/wireframes/Events/events.xlsx
+++ b/design/wireframes/Events/events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Table 1</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Call to action</t>
+  </si>
+  <si>
+    <t>Call to action URL</t>
   </si>
   <si>
     <t>Display until</t>
@@ -107,7 +110,7 @@
     <numFmt numFmtId="59" formatCode="ddd, mmm d, yyyy"/>
     <numFmt numFmtId="60" formatCode="ddd, mmm d, yyyy h:mm AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -119,13 +122,18 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +152,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -157,6 +171,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -170,7 +206,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -179,7 +215,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -188,13 +224,88 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -202,57 +313,59 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -264,60 +377,87 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -336,8 +476,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -356,10 +498,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -553,14 +695,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -575,35 +718,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -856,14 +993,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1152,7 +1295,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1433,204 +1576,235 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.67188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.2969" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.8047" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.60156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.8125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.4219" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.8125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6016" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.3047" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.4219" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.6016" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.6016" style="1" customWidth="1"/>
-    <col min="9" max="256" width="19.6016" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6016" style="1" customWidth="1"/>
+    <col min="10" max="256" width="19.6016" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="6">
         <v>8</v>
+      </c>
+      <c r="I2" t="s" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="80.55" customHeight="1">
-      <c r="A3" s="5">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10">
         <v>41397</v>
       </c>
-      <c r="D3" t="s" s="8">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s" s="9">
+      <c r="D3" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="9">
+      <c r="E3" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="G3" t="s" s="9">
+      <c r="F3" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="G3" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" ht="56.35" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="B4" t="s" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4" s="16">
         <v>41412</v>
       </c>
-      <c r="D4" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="15">
+      <c r="D4" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="F4" t="s" s="15">
+      <c r="E4" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="G4" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" ht="80.35" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13">
+      <c r="B5" t="s" s="15">
+        <v>10</v>
+      </c>
+      <c r="C5" s="16">
         <v>41423</v>
       </c>
-      <c r="D5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s" s="15">
+      <c r="D5" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="F5" t="s" s="15">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16"/>
+      <c r="E5" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s" s="18">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s" s="18">
+        <v>14</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" ht="68.35" customHeight="1">
-      <c r="A6" s="11">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="12">
-        <v>16</v>
-      </c>
-      <c r="C6" s="13">
+      <c r="B6" t="s" s="15">
+        <v>17</v>
+      </c>
+      <c r="C6" s="16">
         <v>41395</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s" s="15">
+      <c r="D6" s="20"/>
+      <c r="E6" t="s" s="18">
         <v>18</v>
       </c>
-      <c r="G6" t="s" s="15">
+      <c r="F6" t="s" s="18">
         <v>19</v>
       </c>
-      <c r="H6" s="16"/>
+      <c r="G6" t="s" s="18">
+        <v>20</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" ht="80.35" customHeight="1">
-      <c r="A7" s="11">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="12">
+      <c r="B7" t="s" s="15">
+        <v>21</v>
+      </c>
+      <c r="C7" s="16">
+        <v>41396</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" t="s" s="18">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s" s="18">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s" s="18">
         <v>20</v>
       </c>
-      <c r="C7" s="13">
-        <v>41396</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s" s="15">
-        <v>19</v>
-      </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" ht="92.35" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="12">
-        <v>22</v>
-      </c>
-      <c r="C8" s="13">
+      <c r="B8" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C8" s="16">
         <v>41471</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" t="s" s="15">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s" s="15">
+      <c r="D8" s="20"/>
+      <c r="E8" t="s" s="18">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s" s="18">
         <v>19</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="G8" t="s" s="18">
+        <v>20</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>